<commit_message>
optimize configuration file for excel
Former-commit-id: 269206afbc3fd0803b5db6a618bee68631289025 [formerly 29a4342be42cbfbb47a62fb5c8020254c3053a18]
Former-commit-id: f7f35cb5d73ec242347805c070073f3dbe69c8dd
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>FilePath</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,24 +74,30 @@
     <t>-0.7,1.5,-1.64</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Stage001</t>
-  </si>
-  <si>
     <t>NewerScene</t>
   </si>
   <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>../../NFDataCfg/Ini/NFZoneServer/Scene/CloneScene/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newscene</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -496,7 +502,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -543,7 +549,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
@@ -558,10 +564,10 @@
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2">
@@ -573,7 +579,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -585,10 +591,10 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3">
@@ -600,7 +606,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -612,10 +618,10 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4">

</xml_diff>

<commit_message>
modified configuration of npc up the bin file of server
Former-commit-id: 8e6f7cc2f709df450f14e86c32b9e4f42bcb5ede [formerly 0d3ed1d624ba30d728200cc617231d46851fee2d]
Former-commit-id: 086344151d4f6c2161ee854ed0d999c60ae690aa
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>FilePath</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,6 +98,14 @@
   </si>
   <si>
     <t>newscene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActorID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CanClone</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -201,9 +209,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I4" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:I4"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K4" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:K4"/>
+  <tableColumns count="11">
     <tableColumn id="1" uniqueName="FilePath" name="FilePath">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@FilePath" xmlDataType="string"/>
     </tableColumn>
@@ -231,6 +239,8 @@
     <tableColumn id="10" uniqueName="Width" name="Width">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@Width" xmlDataType="integer"/>
     </tableColumn>
+    <tableColumn id="6" uniqueName="6" name="CanClone"/>
+    <tableColumn id="11" uniqueName="11" name="ActorID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -499,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -516,9 +526,10 @@
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,8 +557,14 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -573,8 +590,14 @@
       <c r="I2">
         <v>500</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -600,8 +623,14 @@
       <c r="I3">
         <v>500</v>
       </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -626,13 +655,20 @@
       <c r="H4" s="1"/>
       <c r="I4">
         <v>500</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
release v and modified Skill.xml
Former-commit-id: a85134758d1c17b47ebb536a4c3cce12feb81258 [formerly f25da0e38abff81ae34a9601335f26ce736e21a6]
Former-commit-id: ad258019fda0d01acd8d35238bbff1394b7fcbf9
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -107,10 +107,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>186,6.89,88</t>
-  </si>
-  <si>
-    <t>186,6.89,88</t>
+    <t>186,0,88</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>186,0,88</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,7 +522,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
new bin for server
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -81,7 +81,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20,0,60</t>
+    <t>-20,0,-60</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,7 +480,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add loading ui for scene
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>FilePath</t>
   </si>
@@ -116,13 +116,37 @@
   </si>
   <si>
     <t>SelectScene</t>
+  </si>
+  <si>
+    <t>LoadingUI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/ChronoBlade_Caster_wallpaper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>UI/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ChronoBlade_forest_wallpaper</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -132,6 +156,13 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -157,11 +188,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -510,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -525,12 +562,13 @@
     <col min="5" max="5" width="32.375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="27.25" customWidth="1"/>
-    <col min="9" max="9" width="9.375" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="8" max="8" width="38.5" customWidth="1"/>
+    <col min="9" max="9" width="27.25" customWidth="1"/>
+    <col min="10" max="10" width="9.375" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,20 +590,23 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -588,19 +629,22 @@
         <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>500</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
         <v>0</v>
       </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
@@ -620,19 +664,22 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>500</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
         <v>0</v>
       </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>18</v>
@@ -652,20 +699,23 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>500</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
         <v>0</v>
       </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -685,20 +735,23 @@
       <c r="G5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>500</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
         <v>0</v>
       </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -719,19 +772,22 @@
         <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>500</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
         <v>0</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>27</v>
@@ -752,15 +808,18 @@
         <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>500</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add configure for scene
Former-commit-id: 9eaad6122d658f0732e2b46db961a28a801033f5 [formerly b49cdfabe3a558b2ae8f3583e3228b8c41cdd2b9]
Former-commit-id: ae4b17c7576a833a1d1bbdbc9cc442e7a7a54668
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +15,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
-    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Scene" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
   <si>
     <t>FilePath</t>
   </si>
@@ -50,9 +45,18 @@
     <t>SceneShowName</t>
   </si>
   <si>
+    <t>LoadingUI</t>
+  </si>
+  <si>
     <t>SoundList</t>
   </si>
   <si>
+    <t>CamOffestPos</t>
+  </si>
+  <si>
+    <t>CamOffestRot</t>
+  </si>
+  <si>
     <t>Width</t>
   </si>
   <si>
@@ -74,6 +78,18 @@
     <t>villageScene</t>
   </si>
   <si>
+    <t>UI/ChronoBlade_Caster_wallpaper</t>
+  </si>
+  <si>
+    <t>Sources/Music/Town</t>
+  </si>
+  <si>
+    <t>0,8,7</t>
+  </si>
+  <si>
+    <t>45,180</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -92,41 +108,13 @@
     <t>DemoSummer</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>DemoWinter</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>34.10933,1.165174,11.49214</t>
-  </si>
-  <si>
-    <t>Demo2_towers</t>
-  </si>
-  <si>
-    <t>Sources/Music/Town</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SelectScene</t>
-  </si>
-  <si>
-    <t>LoadingUI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI/ChronoBlade_Caster_wallpaper</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>UI/</t>
     </r>
     <r>
@@ -134,19 +122,50 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ChronoBlade_forest_wallpaper</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,-8,7</t>
+  </si>
+  <si>
+    <t>45,0</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>DemoWinter</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>34.10933,1.165174,11.49214</t>
+  </si>
+  <si>
+    <t>Demo2_towers</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>SelectScene</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -154,15 +173,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -183,8 +195,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -192,29 +219,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -513,7 +535,6 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -546,14 +567,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="58.25" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
@@ -563,12 +585,12 @@
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="38.5" customWidth="1"/>
-    <col min="9" max="9" width="27.25" customWidth="1"/>
-    <col min="10" max="10" width="9.375" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="9" max="11" width="27.25" customWidth="1"/>
+    <col min="12" max="12" width="9.375" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,28 +612,34 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>29</v>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -619,34 +647,40 @@
       <c r="D2">
         <v>200</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2">
+        <v>17</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2">
         <v>500</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B3" s="1" t="s">
-        <v>15</v>
+    <row r="3" spans="2:14">
+      <c r="B3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -654,35 +688,41 @@
       <c r="D3">
         <v>200</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3">
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3">
         <v>500</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -690,35 +730,41 @@
       <c r="D4">
         <v>200</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4">
+        <v>500</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4">
-        <v>500</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -726,35 +772,41 @@
       <c r="D5">
         <v>200</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5">
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5">
         <v>500</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -762,35 +814,41 @@
       <c r="D6">
         <v>200</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
+      <c r="E6" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6">
+        <v>35</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6">
         <v>500</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -798,35 +856,40 @@
       <c r="D7">
         <v>200</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7">
+        <v>37</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7">
         <v>500</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 2d act camera
Former-commit-id: a1fbba674a0b0300f20c9b54fbd7328d18abad58 [formerly d4e73ea289d3a3c7c6f337a4cf6ce2e3df800a00]
Former-commit-id: 22cd15e525fd043bcd84942b6e4a52c18e5ceb84
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +15,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
-    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Scene" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
   <si>
     <t>FilePath</t>
   </si>
@@ -89,19 +84,25 @@
     <t>Sources/Music/Town</t>
   </si>
   <si>
+    <t>0,4.2,5.5</t>
+  </si>
+  <si>
+    <t>25,180</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>186,0,88</t>
+  </si>
+  <si>
+    <t>Demo1</t>
+  </si>
+  <si>
     <t>0,8,7</t>
   </si>
   <si>
     <t>45,180</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>186,0,88</t>
-  </si>
-  <si>
-    <t>Demo1</t>
   </si>
   <si>
     <t>3</t>
@@ -133,6 +134,12 @@
     </r>
   </si>
   <si>
+    <t>-7,8,0</t>
+  </si>
+  <si>
+    <t>45,90</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
@@ -152,19 +159,19 @@
   </si>
   <si>
     <t>SelectScene</t>
-  </si>
-  <si>
-    <t>45,90</t>
-  </si>
-  <si>
-    <t>-7,8,0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -172,7 +179,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -194,8 +201,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -213,19 +235,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -524,7 +541,6 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -557,14 +573,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="58.25" customWidth="1"/>
     <col min="2" max="2" width="7.5" customWidth="1"/>
@@ -579,7 +596,7 @@
     <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -667,7 +684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:14">
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
@@ -693,10 +710,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L3">
         <v>500</v>
@@ -708,10 +725,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -720,25 +737,25 @@
         <v>200</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L4">
         <v>500</v>
@@ -750,10 +767,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -762,25 +779,25 @@
         <v>200</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L5">
         <v>500</v>
@@ -792,10 +809,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -804,13 +821,13 @@
         <v>200</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>18</v>
@@ -819,10 +836,10 @@
         <v>19</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L6">
         <v>500</v>
@@ -834,10 +851,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -846,13 +863,13 @@
         <v>200</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>18</v>
@@ -861,10 +878,10 @@
         <v>19</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L7">
         <v>500</v>
@@ -877,8 +894,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed for some error configure file
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -118,6 +118,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>UI/</t>
@@ -127,6 +128,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>ChronoBlade_forest_wallpaper</t>
@@ -187,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -197,6 +199,14 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -584,7 +594,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -851,7 +861,7 @@
         <v>500</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>0</v>

</xml_diff>

<commit_message>
adjust property of scene
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>FilePath</t>
   </si>
@@ -168,18 +168,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0,4.2,5.5</t>
+    <t>0,8,-7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>25,180</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,4.2,-5.5</t>
-  </si>
-  <si>
-    <t>25,0</t>
+    <t>45,0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -583,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -675,10 +668,10 @@
         <v>19</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="L2">
         <v>500</v>
@@ -842,10 +835,10 @@
         <v>19</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L6">
         <v>500</v>

</xml_diff>

<commit_message>
modified born position of city
Former-commit-id: 18f05cf7696e6c9ca1ff2e2ceea5df34512d7b1c [formerly 1dcb8fd23232471c6e38deb4daf9f035f21f1415]
Former-commit-id: a175b5fa24ed4de27e1f72c753229781fcfb4a70
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="19560" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,14 +20,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Scene" type="4" background="1" refreshedVersion="2" saveData="1">
-    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlFormat="all" htmlTables="1"/>
+  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -70,9 +75,6 @@
   </si>
   <si>
     <t>../../NFDataCfg/Ini/NFZoneServer/Scene/PioneerNoob/</t>
-  </si>
-  <si>
-    <t>0,0,0</t>
   </si>
   <si>
     <t>villageScene</t>
@@ -163,18 +165,15 @@
   <si>
     <t>SelectScene</t>
   </si>
+  <si>
+    <t>20,0,-137</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -182,7 +181,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -204,23 +203,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -238,14 +222,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -544,6 +533,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -576,15 +566,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="58.25" customWidth="1"/>
@@ -599,7 +588,7 @@
     <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -657,25 +646,25 @@
         <v>200</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="L2">
         <v>500</v>
@@ -687,9 +676,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -698,25 +687,25 @@
         <v>200</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="L3">
         <v>500</v>
@@ -728,9 +717,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4">
@@ -740,25 +729,25 @@
         <v>200</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="L4">
         <v>500</v>
@@ -770,9 +759,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5">
@@ -782,25 +771,25 @@
         <v>200</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="L5">
         <v>500</v>
@@ -812,9 +801,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6">
@@ -824,25 +813,25 @@
         <v>200</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="L6">
         <v>500</v>
@@ -854,9 +843,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7">
@@ -866,25 +855,25 @@
         <v>200</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="L7">
         <v>500</v>
@@ -897,7 +886,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
reconsitution remove some unused file and code
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -74,9 +74,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>../../NFDataCfg/Ini/NFZoneServer/Scene/PioneerNoob/</t>
-  </si>
-  <si>
     <t>villageScene</t>
   </si>
   <si>
@@ -167,13 +164,142 @@
   </si>
   <si>
     <t>20,0,-137</t>
+  </si>
+  <si>
+    <t>../../NFDataCfg/Ini/Scene/1.xml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../../NFDataCfg/Ini/Scene/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../../NFDataCfg/Ini/Scene/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../../NFDataCfg/Ini/Scene/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../../NFDataCfg/Ini/Scene/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../../NFDataCfg/Ini/Scene/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -183,6 +309,13 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -208,7 +341,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -219,6 +352,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -569,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -637,7 +773,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -646,25 +782,25 @@
         <v>200</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="L2">
         <v>500</v>
@@ -678,7 +814,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -687,25 +826,25 @@
         <v>200</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="L3">
         <v>500</v>
@@ -719,9 +858,11 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C4">
         <v>10</v>
       </c>
@@ -729,25 +870,25 @@
         <v>200</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="L4">
         <v>500</v>
@@ -761,9 +902,11 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C5">
         <v>10</v>
       </c>
@@ -771,25 +914,25 @@
         <v>200</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="L5">
         <v>500</v>
@@ -803,9 +946,11 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C6">
         <v>10</v>
       </c>
@@ -813,25 +958,25 @@
         <v>200</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="L6">
         <v>500</v>
@@ -845,9 +990,11 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C7">
         <v>10</v>
       </c>
@@ -855,25 +1002,25 @@
         <v>200</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="L7">
         <v>500</v>
@@ -888,7 +1035,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add sync property for scene
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView windowWidth="19455" windowHeight="8985"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +15,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
-    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Scene" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47">
   <si>
     <t>ID</t>
   </si>
@@ -71,7 +66,16 @@
     <t>ActorID</t>
   </si>
   <si>
+    <t>Sync</t>
+  </si>
+  <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>../../NFDataCfg/Ini/Scene/1.xml</t>
+  </si>
+  <si>
+    <t>20,0,-137</t>
   </si>
   <si>
     <t>villageScene</t>
@@ -109,68 +113,13 @@
     <t>2</t>
   </si>
   <si>
-    <t>186,0,88</t>
-  </si>
-  <si>
-    <t>Demo1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>28.34387,5.843068,130.1724;133.5562,5.843068,32.58513</t>
-  </si>
-  <si>
-    <t>DemoSummer</t>
-  </si>
-  <si>
-    <t>-7,8,0</t>
-  </si>
-  <si>
-    <t>45,90</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>DemoWinter</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>32.25436,1.283986,20.56763</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>UI/ChronoBlade_Caster_wallpaper</t>
-  </si>
-  <si>
-    <t>0,8,-7</t>
-  </si>
-  <si>
-    <t>45,0</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>34.10933,1.165174,11.49214</t>
-  </si>
-  <si>
-    <t>SelectScene</t>
-  </si>
-  <si>
-    <t>20,0,-137</t>
-  </si>
-  <si>
-    <t>../../NFDataCfg/Ini/Scene/1.xml</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>../../NFDataCfg/Ini/Scene/</t>
     </r>
     <r>
@@ -178,7 +127,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -192,10 +140,24 @@
       </rPr>
       <t>.xml</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>186,0,88</t>
+  </si>
+  <si>
+    <t>Demo1</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>../../NFDataCfg/Ini/Scene/</t>
     </r>
     <r>
@@ -203,7 +165,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -217,10 +178,30 @@
       </rPr>
       <t>.xml</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28.34387,5.843068,130.1724;133.5562,5.843068,32.58513</t>
+  </si>
+  <si>
+    <t>DemoSummer</t>
+  </si>
+  <si>
+    <t>-7,8,0</t>
+  </si>
+  <si>
+    <t>45,90</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>../../NFDataCfg/Ini/Scene/</t>
     </r>
     <r>
@@ -228,7 +209,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -242,10 +222,21 @@
       </rPr>
       <t>.xml</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DemoWinter</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>../../NFDataCfg/Ini/Scene/</t>
     </r>
     <r>
@@ -253,7 +244,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>5</t>
@@ -267,10 +257,33 @@
       </rPr>
       <t>.xml</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32.25436,1.283986,20.56763</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>UI/ChronoBlade_Caster_wallpaper</t>
+  </si>
+  <si>
+    <t>0,8,-7</t>
+  </si>
+  <si>
+    <t>45,0</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>../../NFDataCfg/Ini/Scene/</t>
     </r>
     <r>
@@ -278,7 +291,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>6</t>
@@ -292,14 +304,25 @@
       </rPr>
       <t>.xml</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>34.10933,1.165174,11.49214</t>
+  </si>
+  <si>
+    <t>SelectScene</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -307,27 +330,358 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -335,9 +689,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -354,23 +950,61 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -420,71 +1054,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
         <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -702,14 +1336,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="58.25" customWidth="1"/>
@@ -724,7 +1359,7 @@
     <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -767,13 +1402,16 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -782,25 +1420,25 @@
         <v>200</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L2">
         <v>500</v>
@@ -811,13 +1449,16 @@
       <c r="N2">
         <v>0</v>
       </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -826,25 +1467,25 @@
         <v>200</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="L3">
         <v>500</v>
@@ -855,13 +1496,16 @@
       <c r="N3">
         <v>0</v>
       </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -870,25 +1514,25 @@
         <v>200</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="L4">
         <v>500</v>
@@ -899,13 +1543,16 @@
       <c r="N4">
         <v>0</v>
       </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -914,25 +1561,25 @@
         <v>200</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L5">
         <v>500</v>
@@ -943,13 +1590,16 @@
       <c r="N5">
         <v>0</v>
       </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -958,25 +1608,25 @@
         <v>200</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="L6">
         <v>500</v>
@@ -987,13 +1637,16 @@
       <c r="N6">
         <v>0</v>
       </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1002,25 +1655,25 @@
         <v>200</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L7">
         <v>500</v>
@@ -1031,11 +1684,13 @@
       <c r="N7">
         <v>0</v>
       </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed script for run NF
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherish\Desktop\git\nf\develop\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="13050"/>
+    <workbookView windowWidth="24582" windowHeight="12368"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -20,14 +15,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Scene" type="4" refreshedVersion="2" background="1" saveData="1">
-    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Scene" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Ini\NPC\Scene.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68">
   <si>
     <t>Id</t>
   </si>
@@ -101,6 +96,9 @@
     <t>Ref</t>
   </si>
   <si>
+    <t>Upload</t>
+  </si>
+  <si>
     <t>Desc</t>
   </si>
   <si>
@@ -140,7 +138,7 @@
     <t>villageScene</t>
   </si>
   <si>
-    <t>../../NFDataCfg/Ini/Scene/1.xml</t>
+    <t>../NFDataCfg/Ini/Scene/1.xml</t>
   </si>
   <si>
     <t>12,4,0</t>
@@ -181,33 +179,7 @@
     <t>Demo1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>../../NFDataCfg/Ini/Scene/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>.xml</t>
-    </r>
+    <t>../NFDataCfg/Ini/Scene/2.xml</t>
   </si>
   <si>
     <t>186,0,88</t>
@@ -219,33 +191,7 @@
     <t>DemoSummer</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>../../NFDataCfg/Ini/Scene/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>.xml</t>
-    </r>
+    <t>../NFDataCfg/Ini/Scene/3.xml</t>
   </si>
   <si>
     <t>28.34387,5.843068,130.1724;133.5562,5.843068,32.58513</t>
@@ -263,33 +209,7 @@
     <t>DemoWinter</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>../../NFDataCfg/Ini/Scene/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>.xml</t>
-    </r>
+    <t>../NFDataCfg/Ini/Scene/4.xml</t>
   </si>
   <si>
     <t>5</t>
@@ -298,33 +218,7 @@
     <t>City</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>../../NFDataCfg/Ini/Scene/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>.xml</t>
-    </r>
+    <t>../NFDataCfg/Ini/Scene/5.xml</t>
   </si>
   <si>
     <t>32.25436,1.283986,20.56763</t>
@@ -345,47 +239,23 @@
     <t>SelectScene</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>../../NFDataCfg/Ini/Scene/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>.xml</t>
-    </r>
+    <t>../NFDataCfg/Ini/Scene/6.xml</t>
   </si>
   <si>
     <t>34.10933,1.165174,11.49214</t>
-  </si>
-  <si>
-    <t>Upload</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -400,12 +270,158 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,8 +440,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -549,9 +751,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -599,19 +1043,58 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -938,35 +1421,35 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
   <cols>
-    <col min="1" max="1" width="7.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="1" max="1" width="7.45045045045045" customWidth="1"/>
+    <col min="2" max="2" width="13.7297297297297" customWidth="1"/>
+    <col min="3" max="3" width="12.7297297297297" customWidth="1"/>
+    <col min="4" max="4" width="21.4504504504505" customWidth="1"/>
+    <col min="5" max="5" width="17.0900900900901" customWidth="1"/>
+    <col min="6" max="6" width="31.9459459459459" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" customWidth="1"/>
-    <col min="9" max="11" width="27.26953125" customWidth="1"/>
-    <col min="12" max="12" width="9.36328125" customWidth="1"/>
+    <col min="8" max="8" width="8.90990990990991" customWidth="1"/>
+    <col min="9" max="11" width="27.2702702702703" customWidth="1"/>
+    <col min="12" max="12" width="9.36036036036036" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="13.26953125" customWidth="1"/>
+    <col min="14" max="15" width="13.2702702702703" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:16">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" s="2" customFormat="1" spans="1:16">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -1066,7 +1549,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" s="2" customFormat="1" spans="1:16">
       <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
@@ -1116,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" s="2" customFormat="1" spans="1:16">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -1166,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" s="2" customFormat="1" spans="1:16">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -1216,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" s="2" customFormat="1" spans="1:16">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -1266,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" s="3" customFormat="1" ht="14.15" spans="1:16">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1316,9 +1799,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" s="3" customFormat="1" ht="14.15" spans="1:16">
       <c r="A8" s="9" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -1366,55 +1849,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" s="4" customFormat="1" ht="14.85" spans="1:16">
       <c r="A9" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
       <c r="P9" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" ht="14.15" spans="1:16">
       <c r="A10" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -1423,16 +1906,16 @@
         <v>200</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H10">
         <v>500</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1444,27 +1927,27 @@
         <v>0</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" ht="14.15" spans="1:16">
       <c r="A11" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1473,16 +1956,16 @@
         <v>200</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H11">
         <v>500</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1494,27 +1977,27 @@
         <v>0</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" ht="14.15" spans="1:16">
       <c r="A12" s="12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1523,16 +2006,16 @@
         <v>200</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H12">
         <v>500</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1544,27 +2027,27 @@
         <v>0</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" ht="14.15" spans="1:16">
       <c r="A13" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1573,16 +2056,16 @@
         <v>200</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H13">
         <v>500</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1594,27 +2077,27 @@
         <v>0</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>10</v>
@@ -1623,16 +2106,16 @@
         <v>200</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H14">
         <v>500</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1644,27 +2127,27 @@
         <v>0</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1673,16 +2156,16 @@
         <v>200</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H15">
         <v>500</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1694,27 +2177,26 @@
         <v>0</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O15" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P15">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:P8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed for NFCConsistentHash, NFMemoryCounter and NFCSceneAOIModule
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Scene.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24582" windowHeight="12368"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -370,10 +370,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -392,21 +392,67 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color theme="0"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -414,77 +460,29 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -492,21 +490,38 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -514,29 +529,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -562,7 +562,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,7 +580,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,7 +622,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,7 +658,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,19 +706,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,109 +736,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,35 +872,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -920,7 +891,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -941,21 +927,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -969,153 +940,182 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1164,55 +1164,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -1541,6 +1541,7 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -1549,24 +1550,24 @@
   <sheetPr/>
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K10" sqref="K10:K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="7.45045045045045" customWidth="1"/>
-    <col min="2" max="2" width="13.7297297297297" customWidth="1"/>
-    <col min="3" max="3" width="12.7297297297297" customWidth="1"/>
-    <col min="4" max="4" width="21.4504504504505" customWidth="1"/>
-    <col min="5" max="5" width="17.0900900900901" customWidth="1"/>
-    <col min="6" max="6" width="31.9459459459459" customWidth="1"/>
+    <col min="1" max="1" width="7.45" customWidth="1"/>
+    <col min="2" max="2" width="13.7333333333333" customWidth="1"/>
+    <col min="3" max="3" width="12.7333333333333" customWidth="1"/>
+    <col min="4" max="4" width="21.45" customWidth="1"/>
+    <col min="5" max="5" width="17.0916666666667" customWidth="1"/>
+    <col min="6" max="6" width="31.95" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="8.90990990990991" customWidth="1"/>
-    <col min="9" max="11" width="27.2702702702703" customWidth="1"/>
-    <col min="12" max="12" width="9.36036036036036" customWidth="1"/>
+    <col min="8" max="8" width="8.90833333333333" customWidth="1"/>
+    <col min="9" max="11" width="27.2666666666667" customWidth="1"/>
+    <col min="12" max="12" width="9.35833333333333" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="13.2702702702703" customWidth="1"/>
+    <col min="14" max="15" width="13.2666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:16">
@@ -1869,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="14.15" spans="1:16">
+    <row r="7" s="3" customFormat="1" spans="1:16">
       <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="14.15" spans="1:16">
+    <row r="8" s="3" customFormat="1" spans="1:16">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -1969,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="1" ht="14.85" spans="1:16">
+    <row r="9" s="4" customFormat="1" ht="14.25" spans="1:16">
       <c r="A9" s="10" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +2010,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" ht="14.15" spans="1:16">
+    <row r="10" spans="1:16">
       <c r="A10" s="12" t="s">
         <v>36</v>
       </c>
@@ -2041,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -2059,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="14.15" spans="1:16">
+    <row r="11" spans="1:16">
       <c r="A11" s="12" t="s">
         <v>44</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -2109,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="14.15" spans="1:16">
+    <row r="12" spans="1:16">
       <c r="A12" s="12" t="s">
         <v>48</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -2159,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="14.15" spans="1:16">
+    <row r="13" spans="1:16">
       <c r="A13" s="12" t="s">
         <v>54</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2241,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2291,7 +2292,7 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2341,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2391,7 +2392,7 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2441,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2491,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2541,7 +2542,7 @@
         <v>1</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2591,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2641,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2691,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2741,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2791,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2841,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -2891,7 +2892,7 @@
         <v>1</v>
       </c>
       <c r="K27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -2941,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -2991,7 +2992,7 @@
         <v>1</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -3041,7 +3042,7 @@
         <v>1</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -3091,7 +3092,7 @@
         <v>1</v>
       </c>
       <c r="K31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31">
         <v>0</v>
@@ -3141,7 +3142,7 @@
         <v>1</v>
       </c>
       <c r="K32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -3191,7 +3192,7 @@
         <v>1</v>
       </c>
       <c r="K33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33">
         <v>0</v>
@@ -3241,7 +3242,7 @@
         <v>1</v>
       </c>
       <c r="K34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -3291,7 +3292,7 @@
         <v>1</v>
       </c>
       <c r="K35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35">
         <v>0</v>

</xml_diff>